<commit_message>
feat: turn web bubble chart to only timeline
</commit_message>
<xml_diff>
--- a/wit/web_region_bubble/travel_market_summary.xlsx
+++ b/wit/web_region_bubble/travel_market_summary.xlsx
@@ -5,23 +5,26 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/130fda80f0432a83/TravelMarketViz/wit/web_region_bubble/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/130fda80f0432a83/TravelMarketViz/wit/web_region_bubble_MENA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_4566CFE2356CD672DB3B3595395BDA16D654840E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FD62608-A5D8-7A42-A439-0EF2511E137C}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_4566CFE2356CD672DB3B3595395BDA16D654840E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30415E5F-E6C7-B741-9F2A-E081442BE8A2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="2920" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualization Data" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Visualization Data'!$B$1:$B$921</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15630" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15708" uniqueCount="66">
   <si>
     <t>Year</t>
   </si>
@@ -275,11 +278,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,15 +590,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F882"/>
+  <dimension ref="A1:F921"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="134" workbookViewId="0">
-      <selection activeCell="F161" sqref="F161"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -18237,7 +18243,788 @@
         <v>64.09</v>
       </c>
     </row>
+    <row r="883" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A883" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B883" t="s">
+        <v>8</v>
+      </c>
+      <c r="C883" t="s">
+        <v>7</v>
+      </c>
+      <c r="D883" s="2">
+        <v>61801952418</v>
+      </c>
+      <c r="E883" s="2">
+        <v>3901056597</v>
+      </c>
+      <c r="F883">
+        <v>6.31</v>
+      </c>
+    </row>
+    <row r="884" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A884" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B884" t="s">
+        <v>9</v>
+      </c>
+      <c r="C884" t="s">
+        <v>7</v>
+      </c>
+      <c r="D884" s="2">
+        <v>9120168879</v>
+      </c>
+      <c r="E884" s="2">
+        <v>532560975</v>
+      </c>
+      <c r="F884">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="885" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A885" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B885" t="s">
+        <v>10</v>
+      </c>
+      <c r="C885" t="s">
+        <v>7</v>
+      </c>
+      <c r="D885" s="2">
+        <v>17216829245</v>
+      </c>
+      <c r="E885" s="2">
+        <v>3493055529</v>
+      </c>
+      <c r="F885">
+        <v>20.29</v>
+      </c>
+    </row>
+    <row r="886" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A886" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B886" t="s">
+        <v>11</v>
+      </c>
+      <c r="C886" t="s">
+        <v>7</v>
+      </c>
+      <c r="D886" s="2">
+        <v>4973584490</v>
+      </c>
+      <c r="E886" s="2">
+        <v>150211616</v>
+      </c>
+      <c r="F886">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="887" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A887" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B887" t="s">
+        <v>12</v>
+      </c>
+      <c r="C887" t="s">
+        <v>7</v>
+      </c>
+      <c r="D887" s="2">
+        <v>86924413735</v>
+      </c>
+      <c r="E887" s="2">
+        <v>20473209528</v>
+      </c>
+      <c r="F887">
+        <v>23.55</v>
+      </c>
+    </row>
+    <row r="888" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A888" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B888" t="s">
+        <v>13</v>
+      </c>
+      <c r="C888" t="s">
+        <v>7</v>
+      </c>
+      <c r="D888" s="2">
+        <v>564118907</v>
+      </c>
+      <c r="E888" s="2">
+        <v>12968842</v>
+      </c>
+      <c r="F888">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="889" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A889" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B889" t="s">
+        <v>14</v>
+      </c>
+      <c r="C889" t="s">
+        <v>7</v>
+      </c>
+      <c r="D889" s="2">
+        <v>5378207637</v>
+      </c>
+      <c r="E889" s="2">
+        <v>1334952055</v>
+      </c>
+      <c r="F889">
+        <v>24.82</v>
+      </c>
+    </row>
+    <row r="890" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A890" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B890" t="s">
+        <v>15</v>
+      </c>
+      <c r="C890" t="s">
+        <v>7</v>
+      </c>
+      <c r="D890" s="2">
+        <v>6744239871</v>
+      </c>
+      <c r="E890" s="2">
+        <v>1560905054</v>
+      </c>
+      <c r="F890">
+        <v>23.14</v>
+      </c>
+    </row>
+    <row r="891" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A891" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B891" t="s">
+        <v>16</v>
+      </c>
+      <c r="C891" t="s">
+        <v>7</v>
+      </c>
+      <c r="D891" s="2">
+        <v>10017846982</v>
+      </c>
+      <c r="E891" s="2">
+        <v>1190618080</v>
+      </c>
+      <c r="F891">
+        <v>11.88</v>
+      </c>
+    </row>
+    <row r="892" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A892" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B892" t="s">
+        <v>17</v>
+      </c>
+      <c r="C892" t="s">
+        <v>7</v>
+      </c>
+      <c r="D892" s="2">
+        <v>4690947283</v>
+      </c>
+      <c r="E892" s="2">
+        <v>439478770</v>
+      </c>
+      <c r="F892">
+        <v>9.3699999999999992</v>
+      </c>
+    </row>
+    <row r="893" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A893" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B893" t="s">
+        <v>18</v>
+      </c>
+      <c r="C893" t="s">
+        <v>7</v>
+      </c>
+      <c r="D893" s="2">
+        <v>9455109359</v>
+      </c>
+      <c r="E893" s="2">
+        <v>1240271588</v>
+      </c>
+      <c r="F893">
+        <v>13.12</v>
+      </c>
+    </row>
+    <row r="894" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A894" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B894" t="s">
+        <v>19</v>
+      </c>
+      <c r="C894" t="s">
+        <v>20</v>
+      </c>
+      <c r="D894" s="2">
+        <v>1417855507</v>
+      </c>
+      <c r="E894" s="2">
+        <v>99515468</v>
+      </c>
+      <c r="F894">
+        <v>7.02</v>
+      </c>
+    </row>
+    <row r="895" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A895" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B895" t="s">
+        <v>21</v>
+      </c>
+      <c r="C895" t="s">
+        <v>20</v>
+      </c>
+      <c r="D895" s="2">
+        <v>3158693808</v>
+      </c>
+      <c r="E895" s="2">
+        <v>485330141</v>
+      </c>
+      <c r="F895">
+        <v>15.36</v>
+      </c>
+    </row>
+    <row r="896" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A896" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B896" t="s">
+        <v>22</v>
+      </c>
+      <c r="C896" t="s">
+        <v>20</v>
+      </c>
+      <c r="D896" s="2">
+        <v>10274475285</v>
+      </c>
+      <c r="E896" s="2">
+        <v>2068025188</v>
+      </c>
+      <c r="F896">
+        <v>20.13</v>
+      </c>
+    </row>
+    <row r="897" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A897" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B897" t="s">
+        <v>23</v>
+      </c>
+      <c r="C897" t="s">
+        <v>20</v>
+      </c>
+      <c r="D897" s="2">
+        <v>2541454383</v>
+      </c>
+      <c r="E897" s="2">
+        <v>466876316</v>
+      </c>
+      <c r="F897">
+        <v>18.37</v>
+      </c>
+    </row>
+    <row r="898" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A898" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B898" t="s">
+        <v>24</v>
+      </c>
+      <c r="C898" t="s">
+        <v>20</v>
+      </c>
+      <c r="D898" s="2">
+        <v>3837150854</v>
+      </c>
+      <c r="E898" s="2">
+        <v>617507857</v>
+      </c>
+      <c r="F898">
+        <v>16.09</v>
+      </c>
+    </row>
+    <row r="899" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A899" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B899" t="s">
+        <v>25</v>
+      </c>
+      <c r="C899" t="s">
+        <v>20</v>
+      </c>
+      <c r="D899" s="2">
+        <v>2888012700</v>
+      </c>
+      <c r="E899" s="2">
+        <v>270270445</v>
+      </c>
+      <c r="F899">
+        <v>9.36</v>
+      </c>
+    </row>
+    <row r="900" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A900" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B900" t="s">
+        <v>26</v>
+      </c>
+      <c r="C900" t="s">
+        <v>20</v>
+      </c>
+      <c r="D900" s="2">
+        <v>3264309519</v>
+      </c>
+      <c r="E900" s="2">
+        <v>371903179</v>
+      </c>
+      <c r="F900">
+        <v>11.39</v>
+      </c>
+    </row>
+    <row r="901" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A901" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B901" t="s">
+        <v>27</v>
+      </c>
+      <c r="C901" t="s">
+        <v>20</v>
+      </c>
+      <c r="D901" s="2">
+        <v>35070527360</v>
+      </c>
+      <c r="E901" s="2">
+        <v>2008822094</v>
+      </c>
+      <c r="F901">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="902" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A902" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B902" t="s">
+        <v>28</v>
+      </c>
+      <c r="C902" t="s">
+        <v>20</v>
+      </c>
+      <c r="D902" s="2">
+        <v>3461034991</v>
+      </c>
+      <c r="E902" s="2">
+        <v>428082317</v>
+      </c>
+      <c r="F902">
+        <v>12.37</v>
+      </c>
+    </row>
+    <row r="903" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A903" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B903" t="s">
+        <v>29</v>
+      </c>
+      <c r="C903" t="s">
+        <v>30</v>
+      </c>
+      <c r="D903" s="2">
+        <v>52159785888</v>
+      </c>
+      <c r="E903" s="2">
+        <v>15112333104</v>
+      </c>
+      <c r="F903">
+        <v>28.97</v>
+      </c>
+    </row>
+    <row r="904" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A904" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B904" t="s">
+        <v>31</v>
+      </c>
+      <c r="C904" t="s">
+        <v>30</v>
+      </c>
+      <c r="D904" s="2">
+        <v>65830765918</v>
+      </c>
+      <c r="E904" s="2">
+        <v>18498339972</v>
+      </c>
+      <c r="F904">
+        <v>28.1</v>
+      </c>
+    </row>
+    <row r="905" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A905" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B905" t="s">
+        <v>32</v>
+      </c>
+      <c r="C905" t="s">
+        <v>30</v>
+      </c>
+      <c r="D905" s="2">
+        <v>25565414400</v>
+      </c>
+      <c r="E905" s="2">
+        <v>5229101223</v>
+      </c>
+      <c r="F905">
+        <v>20.45</v>
+      </c>
+    </row>
+    <row r="906" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A906" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B906" t="s">
+        <v>33</v>
+      </c>
+      <c r="C906" t="s">
+        <v>30</v>
+      </c>
+      <c r="D906" s="2">
+        <v>56689701816</v>
+      </c>
+      <c r="E906" s="2">
+        <v>13840131136</v>
+      </c>
+      <c r="F906">
+        <v>24.41</v>
+      </c>
+    </row>
+    <row r="907" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A907" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B907" t="s">
+        <v>34</v>
+      </c>
+      <c r="C907" t="s">
+        <v>30</v>
+      </c>
+      <c r="D907" s="2">
+        <v>17527588226</v>
+      </c>
+      <c r="E907" s="2">
+        <v>6346787240</v>
+      </c>
+      <c r="F907">
+        <v>36.21</v>
+      </c>
+    </row>
+    <row r="908" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A908" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B908" t="s">
+        <v>35</v>
+      </c>
+      <c r="C908" t="s">
+        <v>30</v>
+      </c>
+      <c r="D908" s="2">
+        <v>26478097443</v>
+      </c>
+      <c r="E908" s="2">
+        <v>5512486843</v>
+      </c>
+      <c r="F908">
+        <v>20.82</v>
+      </c>
+    </row>
+    <row r="909" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A909" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B909" t="s">
+        <v>36</v>
+      </c>
+      <c r="C909" t="s">
+        <v>30</v>
+      </c>
+      <c r="D909" s="2">
+        <v>54400813036</v>
+      </c>
+      <c r="E909" s="2">
+        <v>18072444293</v>
+      </c>
+      <c r="F909">
+        <v>33.22</v>
+      </c>
+    </row>
+    <row r="910" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A910" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B910" t="s">
+        <v>37</v>
+      </c>
+      <c r="C910" t="s">
+        <v>38</v>
+      </c>
+      <c r="D910" s="2">
+        <v>9134756610</v>
+      </c>
+      <c r="E910" s="2">
+        <v>411951945</v>
+      </c>
+      <c r="F910">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="911" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A911" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B911" t="s">
+        <v>39</v>
+      </c>
+      <c r="C911" t="s">
+        <v>38</v>
+      </c>
+      <c r="D911" s="2">
+        <v>40495595841</v>
+      </c>
+      <c r="E911" s="2">
+        <v>4125220696</v>
+      </c>
+      <c r="F911">
+        <v>10.19</v>
+      </c>
+    </row>
+    <row r="912" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A912" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B912" t="s">
+        <v>40</v>
+      </c>
+      <c r="C912" t="s">
+        <v>38</v>
+      </c>
+      <c r="D912" s="2">
+        <v>4575854253</v>
+      </c>
+      <c r="E912" s="2">
+        <v>776242064</v>
+      </c>
+      <c r="F912">
+        <v>16.96</v>
+      </c>
+    </row>
+    <row r="913" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A913" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B913" t="s">
+        <v>41</v>
+      </c>
+      <c r="C913" t="s">
+        <v>38</v>
+      </c>
+      <c r="D913" s="2">
+        <v>8326390288</v>
+      </c>
+      <c r="E913" s="2">
+        <v>554673116</v>
+      </c>
+      <c r="F913">
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="914" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A914" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B914" t="s">
+        <v>42</v>
+      </c>
+      <c r="C914" t="s">
+        <v>38</v>
+      </c>
+      <c r="D914" s="2">
+        <v>18850009623</v>
+      </c>
+      <c r="E914" s="2">
+        <v>2683764576</v>
+      </c>
+      <c r="F914">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="915" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A915" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B915" t="s">
+        <v>43</v>
+      </c>
+      <c r="C915" t="s">
+        <v>44</v>
+      </c>
+      <c r="D915" s="2">
+        <v>8092418672</v>
+      </c>
+      <c r="E915" s="2">
+        <v>450101676</v>
+      </c>
+      <c r="F915">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="916" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A916" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B916" t="s">
+        <v>45</v>
+      </c>
+      <c r="C916" t="s">
+        <v>44</v>
+      </c>
+      <c r="D916" s="2">
+        <v>5148813911</v>
+      </c>
+      <c r="E916" s="2">
+        <v>797228443</v>
+      </c>
+      <c r="F916">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="917" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A917" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B917" t="s">
+        <v>46</v>
+      </c>
+      <c r="C917" t="s">
+        <v>44</v>
+      </c>
+      <c r="D917" s="2">
+        <v>7629640786</v>
+      </c>
+      <c r="E917" s="2">
+        <v>575826744</v>
+      </c>
+      <c r="F917">
+        <v>7.55</v>
+      </c>
+    </row>
+    <row r="918" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A918" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B918" t="s">
+        <v>47</v>
+      </c>
+      <c r="C918" t="s">
+        <v>44</v>
+      </c>
+      <c r="D918" s="2">
+        <v>9206319269</v>
+      </c>
+      <c r="E918" s="2">
+        <v>996882925</v>
+      </c>
+      <c r="F918">
+        <v>10.83</v>
+      </c>
+    </row>
+    <row r="919" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A919" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B919" t="s">
+        <v>48</v>
+      </c>
+      <c r="C919" t="s">
+        <v>44</v>
+      </c>
+      <c r="D919" s="2">
+        <v>21023683070</v>
+      </c>
+      <c r="E919" s="2">
+        <v>3044136383</v>
+      </c>
+      <c r="F919">
+        <v>14.48</v>
+      </c>
+    </row>
+    <row r="920" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A920" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B920" t="s">
+        <v>49</v>
+      </c>
+      <c r="C920" t="s">
+        <v>50</v>
+      </c>
+      <c r="D920" s="2">
+        <v>23278233995</v>
+      </c>
+      <c r="E920" s="2">
+        <v>8387571252</v>
+      </c>
+      <c r="F920">
+        <v>36.03</v>
+      </c>
+    </row>
+    <row r="921" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A921" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B921" t="s">
+        <v>51</v>
+      </c>
+      <c r="C921" t="s">
+        <v>50</v>
+      </c>
+      <c r="D921" s="2">
+        <v>231979443474</v>
+      </c>
+      <c r="E921" s="2">
+        <v>89779576556</v>
+      </c>
+      <c r="F921">
+        <v>38.700000000000003</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="B1:B921" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>